<commit_message>
Adding figures/tables and updated code
Recreated figures/tables from Kim et al., updating code to reflect this
</commit_message>
<xml_diff>
--- a/Assignment 1/Data_Codebook.xlsx
+++ b/Assignment 1/Data_Codebook.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="92">
   <si>
     <t>Variable</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t>Glutamic pyruvic transaminase (ALT)</t>
+  </si>
+  <si>
+    <t>MS_5cri</t>
+  </si>
+  <si>
+    <t>Number of criteria met for metabolic syndrome diagnosis</t>
   </si>
   <si>
     <t>The FREQ Procedure</t>
@@ -544,7 +550,7 @@
   <sheetPr filterMode="0" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
     </sheetView>
@@ -552,7 +558,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="32.71" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.71" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.71" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.71" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.71" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.71" bestFit="1" customWidth="1"/>
@@ -669,7 +675,7 @@
         <v>23.7068002936858</v>
       </c>
       <c r="G4" s="5">
-        <v>3.4157648034963</v>
+        <v>3.41576480349629</v>
       </c>
       <c r="H4" s="5">
         <v>14.3</v>
@@ -811,7 +817,7 @@
         <v>88.2</v>
       </c>
       <c r="F9" s="5">
-        <v>91.4851104698973</v>
+        <v>91.4851104698972</v>
       </c>
       <c r="G9" s="5">
         <v>35.198330207156</v>
@@ -869,7 +875,7 @@
         <v>19.725</v>
       </c>
       <c r="F11" s="5">
-        <v>19.8085950477974</v>
+        <v>19.8085950477973</v>
       </c>
       <c r="G11" s="5">
         <v>4.855155508551</v>
@@ -1043,7 +1049,7 @@
         <v>5.1</v>
       </c>
       <c r="F17" s="5">
-        <v>5.24509877003355</v>
+        <v>5.24509877003354</v>
       </c>
       <c r="G17" s="5">
         <v>1.33637772188318</v>
@@ -1104,7 +1110,7 @@
         <v>9.65114754098361</v>
       </c>
       <c r="G19" s="5">
-        <v>5.77707074356773</v>
+        <v>5.77707074356774</v>
       </c>
       <c r="H19" s="5">
         <v>1.7</v>
@@ -1133,7 +1139,7 @@
         <v>0.14858516886931</v>
       </c>
       <c r="G20" s="5">
-        <v>0.46119764760056</v>
+        <v>0.46119764760055</v>
       </c>
       <c r="H20" s="5">
         <v>0.02</v>
@@ -1162,7 +1168,7 @@
         <v>29.9354740975044</v>
       </c>
       <c r="G21" s="5">
-        <v>3.62511332237539</v>
+        <v>3.62511332237538</v>
       </c>
       <c r="H21" s="5">
         <v>16.54624277</v>
@@ -1191,7 +1197,7 @@
         <v>2.42393442622951</v>
       </c>
       <c r="G22" s="5">
-        <v>1.64728552502264</v>
+        <v>1.64728552502263</v>
       </c>
       <c r="H22" s="5">
         <v>0.36</v>
@@ -1258,486 +1264,498 @@
         <v>1209</v>
       </c>
     </row>
-    <row r="25" ht="12" customHeight="1"/>
-    <row r="26" ht="14" customHeight="1">
-      <c r="A26" s="6" t="s">
+    <row r="25" ht="14" customHeight="1">
+      <c r="A25" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="27" ht="12" customHeight="1"/>
-    <row r="28" ht="14" customHeight="1">
-      <c r="A28" s="7" t="s">
+      <c r="B25" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29" ht="29" customHeight="1">
-      <c r="A29" s="8" t="s">
+      <c r="C25" s="4">
+        <v>13620</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
+        <v>1</v>
+      </c>
+      <c r="F25" s="5">
+        <v>1.22936857562408</v>
+      </c>
+      <c r="G25" s="5">
+        <v>1.22044929457708</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0</v>
+      </c>
+      <c r="I25" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" ht="12" customHeight="1"/>
+    <row r="27" ht="14" customHeight="1">
+      <c r="A27" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="8" t="s">
+    </row>
+    <row r="28" ht="12" customHeight="1"/>
+    <row r="29" ht="14" customHeight="1">
+      <c r="A29" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+    </row>
+    <row r="30" ht="29" customHeight="1">
+      <c r="A30" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="C30" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="30" ht="14" customHeight="1">
-      <c r="A30" s="2" t="s">
+      <c r="D30" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="10">
-        <v>7422</v>
-      </c>
-      <c r="C30" s="11">
-        <v>54.49</v>
-      </c>
-      <c r="D30" s="10">
-        <v>7422</v>
-      </c>
-      <c r="E30" s="11">
-        <v>54.49</v>
+      <c r="E30" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="31" ht="14" customHeight="1">
       <c r="A31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="10">
+        <v>7422</v>
+      </c>
+      <c r="C31" s="11">
+        <v>54.49</v>
+      </c>
+      <c r="D31" s="10">
+        <v>7422</v>
+      </c>
+      <c r="E31" s="11">
+        <v>54.49</v>
+      </c>
+    </row>
+    <row r="32" ht="14" customHeight="1">
+      <c r="A32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="10">
+        <v>6198</v>
+      </c>
+      <c r="C32" s="11">
+        <v>45.51</v>
+      </c>
+      <c r="D32" s="10">
+        <v>13620</v>
+      </c>
+      <c r="E32" s="11">
+        <v>100.00</v>
+      </c>
+    </row>
+    <row r="33" ht="12" customHeight="1"/>
+    <row r="34" ht="14" customHeight="1">
+      <c r="A34" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+    </row>
+    <row r="35" ht="29" customHeight="1">
+      <c r="A35" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="B31" s="10">
-        <v>6198</v>
-      </c>
-      <c r="C31" s="11">
-        <v>45.51</v>
-      </c>
-      <c r="D31" s="10">
-        <v>13620</v>
-      </c>
-      <c r="E31" s="11">
-        <v>100.00</v>
-      </c>
-    </row>
-    <row r="32" ht="12" customHeight="1"/>
-    <row r="33" ht="14" customHeight="1">
-      <c r="A33" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-    </row>
-    <row r="34" ht="29" customHeight="1">
-      <c r="A34" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" ht="14" customHeight="1">
-      <c r="A35" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="10">
-        <v>11382</v>
-      </c>
-      <c r="C35" s="11">
-        <v>83.57</v>
-      </c>
-      <c r="D35" s="10">
-        <v>11382</v>
-      </c>
-      <c r="E35" s="11">
-        <v>83.57</v>
       </c>
     </row>
     <row r="36" ht="14" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B36" s="10">
+        <v>11382</v>
+      </c>
+      <c r="C36" s="11">
+        <v>83.57</v>
+      </c>
+      <c r="D36" s="10">
+        <v>11382</v>
+      </c>
+      <c r="E36" s="11">
+        <v>83.57</v>
+      </c>
+    </row>
+    <row r="37" ht="14" customHeight="1">
+      <c r="A37" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="10">
         <v>2238</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C37" s="11">
         <v>16.43</v>
       </c>
-      <c r="D36" s="10">
-        <v>13620</v>
-      </c>
-      <c r="E36" s="11">
+      <c r="D37" s="10">
+        <v>13620</v>
+      </c>
+      <c r="E37" s="11">
         <v>100.00</v>
       </c>
     </row>
-    <row r="37" ht="12" customHeight="1"/>
-    <row r="38" ht="14" customHeight="1">
-      <c r="A38" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-    </row>
-    <row r="39" ht="29" customHeight="1">
-      <c r="A39" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D39" s="9" t="s">
+    <row r="38" ht="12" customHeight="1"/>
+    <row r="39" ht="14" customHeight="1">
+      <c r="A39" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+    </row>
+    <row r="40" ht="29" customHeight="1">
+      <c r="A40" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="C40" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="40" ht="14" customHeight="1">
-      <c r="A40" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B40" s="10">
-        <v>9390</v>
-      </c>
-      <c r="C40" s="11">
-        <v>68.94</v>
-      </c>
-      <c r="D40" s="10">
-        <v>9390</v>
-      </c>
-      <c r="E40" s="11">
-        <v>68.94</v>
+      <c r="D40" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="41" ht="14" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B41" s="10">
+        <v>9390</v>
+      </c>
+      <c r="C41" s="11">
+        <v>68.94</v>
+      </c>
+      <c r="D41" s="10">
+        <v>9390</v>
+      </c>
+      <c r="E41" s="11">
+        <v>68.94</v>
+      </c>
+    </row>
+    <row r="42" ht="14" customHeight="1">
+      <c r="A42" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="10">
         <v>4230</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C42" s="11">
         <v>31.06</v>
       </c>
-      <c r="D41" s="10">
-        <v>13620</v>
-      </c>
-      <c r="E41" s="11">
+      <c r="D42" s="10">
+        <v>13620</v>
+      </c>
+      <c r="E42" s="11">
         <v>100.00</v>
       </c>
     </row>
-    <row r="42" ht="12" customHeight="1"/>
-    <row r="43" ht="14" customHeight="1">
-      <c r="A43" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-    </row>
-    <row r="44" ht="29" customHeight="1">
-      <c r="A44" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D44" s="9" t="s">
+    <row r="43" ht="12" customHeight="1"/>
+    <row r="44" ht="14" customHeight="1">
+      <c r="A44" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+    </row>
+    <row r="45" ht="29" customHeight="1">
+      <c r="A45" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="C45" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="45" ht="14" customHeight="1">
-      <c r="A45" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B45" s="10">
-        <v>12481</v>
-      </c>
-      <c r="C45" s="11">
-        <v>91.64</v>
-      </c>
-      <c r="D45" s="10">
-        <v>12481</v>
-      </c>
-      <c r="E45" s="11">
-        <v>91.64</v>
+      <c r="D45" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="46" ht="14" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B46" s="10">
+        <v>12481</v>
+      </c>
+      <c r="C46" s="11">
+        <v>91.64</v>
+      </c>
+      <c r="D46" s="10">
+        <v>12481</v>
+      </c>
+      <c r="E46" s="11">
+        <v>91.64</v>
+      </c>
+    </row>
+    <row r="47" ht="14" customHeight="1">
+      <c r="A47" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="10">
         <v>1139</v>
       </c>
-      <c r="C46" s="11">
+      <c r="C47" s="11">
         <v>8.36</v>
       </c>
-      <c r="D46" s="10">
-        <v>13620</v>
-      </c>
-      <c r="E46" s="11">
+      <c r="D47" s="10">
+        <v>13620</v>
+      </c>
+      <c r="E47" s="11">
         <v>100.00</v>
       </c>
     </row>
-    <row r="47" ht="12" customHeight="1"/>
-    <row r="48" ht="14" customHeight="1">
-      <c r="A48" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-    </row>
-    <row r="49" ht="29" customHeight="1">
-      <c r="A49" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D49" s="9" t="s">
+    <row r="48" ht="12" customHeight="1"/>
+    <row r="49" ht="14" customHeight="1">
+      <c r="A49" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+    </row>
+    <row r="50" ht="29" customHeight="1">
+      <c r="A50" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E49" s="9" t="s">
+      <c r="C50" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="50" ht="14" customHeight="1">
-      <c r="A50" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B50" s="10">
-        <v>11239</v>
-      </c>
-      <c r="C50" s="11">
-        <v>82.52</v>
-      </c>
-      <c r="D50" s="10">
-        <v>11239</v>
-      </c>
-      <c r="E50" s="11">
-        <v>82.52</v>
+      <c r="D50" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="51" ht="14" customHeight="1">
       <c r="A51" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B51" s="10">
+        <v>11239</v>
+      </c>
+      <c r="C51" s="11">
+        <v>82.52</v>
+      </c>
+      <c r="D51" s="10">
+        <v>11239</v>
+      </c>
+      <c r="E51" s="11">
+        <v>82.52</v>
+      </c>
+    </row>
+    <row r="52" ht="14" customHeight="1">
+      <c r="A52" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" s="10">
         <v>2381</v>
       </c>
-      <c r="C51" s="11">
+      <c r="C52" s="11">
         <v>17.48</v>
       </c>
-      <c r="D51" s="10">
-        <v>13620</v>
-      </c>
-      <c r="E51" s="11">
+      <c r="D52" s="10">
+        <v>13620</v>
+      </c>
+      <c r="E52" s="11">
         <v>100.00</v>
       </c>
     </row>
-    <row r="52" ht="12" customHeight="1"/>
-    <row r="53" ht="14" customHeight="1">
-      <c r="A53" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-    </row>
-    <row r="54" ht="29" customHeight="1">
-      <c r="A54" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D54" s="9" t="s">
+    <row r="53" ht="12" customHeight="1"/>
+    <row r="54" ht="14" customHeight="1">
+      <c r="A54" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+    </row>
+    <row r="55" ht="29" customHeight="1">
+      <c r="A55" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E54" s="9" t="s">
+      <c r="C55" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="55" ht="14" customHeight="1">
-      <c r="A55" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B55" s="10">
-        <v>6396</v>
-      </c>
-      <c r="C55" s="11">
-        <v>46.96</v>
-      </c>
-      <c r="D55" s="10">
-        <v>6396</v>
-      </c>
-      <c r="E55" s="11">
-        <v>46.96</v>
+      <c r="D55" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="56" ht="14" customHeight="1">
       <c r="A56" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B56" s="10">
+        <v>6396</v>
+      </c>
+      <c r="C56" s="11">
+        <v>46.96</v>
+      </c>
+      <c r="D56" s="10">
+        <v>6396</v>
+      </c>
+      <c r="E56" s="11">
+        <v>46.96</v>
+      </c>
+    </row>
+    <row r="57" ht="14" customHeight="1">
+      <c r="A57" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" s="10">
         <v>7224</v>
       </c>
-      <c r="C56" s="11">
+      <c r="C57" s="11">
         <v>53.04</v>
       </c>
-      <c r="D56" s="10">
-        <v>13620</v>
-      </c>
-      <c r="E56" s="11">
+      <c r="D57" s="10">
+        <v>13620</v>
+      </c>
+      <c r="E57" s="11">
         <v>100.00</v>
       </c>
     </row>
-    <row r="57" ht="12" customHeight="1"/>
-    <row r="58" ht="14" customHeight="1">
-      <c r="A58" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-    </row>
-    <row r="59" ht="29" customHeight="1">
-      <c r="A59" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D59" s="9" t="s">
+    <row r="58" ht="12" customHeight="1"/>
+    <row r="59" ht="14" customHeight="1">
+      <c r="A59" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+    </row>
+    <row r="60" ht="29" customHeight="1">
+      <c r="A60" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B60" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E59" s="9" t="s">
+      <c r="C60" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="60" ht="14" customHeight="1">
-      <c r="A60" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B60" s="10">
-        <v>8549</v>
-      </c>
-      <c r="C60" s="11">
-        <v>62.77</v>
-      </c>
-      <c r="D60" s="10">
-        <v>8549</v>
-      </c>
-      <c r="E60" s="11">
-        <v>62.77</v>
+      <c r="D60" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="61" ht="14" customHeight="1">
       <c r="A61" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B61" s="10">
+        <v>8549</v>
+      </c>
+      <c r="C61" s="11">
+        <v>62.77</v>
+      </c>
+      <c r="D61" s="10">
+        <v>8549</v>
+      </c>
+      <c r="E61" s="11">
+        <v>62.77</v>
+      </c>
+    </row>
+    <row r="62" ht="14" customHeight="1">
+      <c r="A62" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" s="10">
         <v>5071</v>
       </c>
-      <c r="C61" s="11">
+      <c r="C62" s="11">
         <v>37.23</v>
       </c>
-      <c r="D61" s="10">
-        <v>13620</v>
-      </c>
-      <c r="E61" s="11">
+      <c r="D62" s="10">
+        <v>13620</v>
+      </c>
+      <c r="E62" s="11">
         <v>100.00</v>
       </c>
     </row>
-    <row r="62" ht="12" customHeight="1"/>
-    <row r="63" ht="14" customHeight="1">
-      <c r="A63" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-    </row>
-    <row r="64" ht="29" customHeight="1">
-      <c r="A64" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D64" s="9" t="s">
+    <row r="63" ht="12" customHeight="1"/>
+    <row r="64" ht="14" customHeight="1">
+      <c r="A64" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+    </row>
+    <row r="65" ht="29" customHeight="1">
+      <c r="A65" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B65" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E64" s="9" t="s">
+      <c r="C65" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="65" ht="14" customHeight="1">
-      <c r="A65" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B65" s="10">
-        <v>3405</v>
-      </c>
-      <c r="C65" s="11">
-        <v>25.00</v>
-      </c>
-      <c r="D65" s="10">
-        <v>3405</v>
-      </c>
-      <c r="E65" s="11">
-        <v>25.00</v>
+      <c r="D65" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="66" ht="14" customHeight="1">
       <c r="A66" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B66" s="10">
         <v>3405</v>
@@ -1746,15 +1764,15 @@
         <v>25.00</v>
       </c>
       <c r="D66" s="10">
-        <v>6810</v>
+        <v>3405</v>
       </c>
       <c r="E66" s="11">
-        <v>50.00</v>
+        <v>25.00</v>
       </c>
     </row>
     <row r="67" ht="14" customHeight="1">
       <c r="A67" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B67" s="10">
         <v>3405</v>
@@ -1763,15 +1781,15 @@
         <v>25.00</v>
       </c>
       <c r="D67" s="10">
-        <v>10215</v>
+        <v>6810</v>
       </c>
       <c r="E67" s="11">
-        <v>75.00</v>
+        <v>50.00</v>
       </c>
     </row>
     <row r="68" ht="14" customHeight="1">
       <c r="A68" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B68" s="10">
         <v>3405</v>
@@ -1780,182 +1798,199 @@
         <v>25.00</v>
       </c>
       <c r="D68" s="10">
-        <v>13620</v>
+        <v>10215</v>
       </c>
       <c r="E68" s="11">
+        <v>75.00</v>
+      </c>
+    </row>
+    <row r="69" ht="14" customHeight="1">
+      <c r="A69" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B69" s="10">
+        <v>3405</v>
+      </c>
+      <c r="C69" s="11">
+        <v>25.00</v>
+      </c>
+      <c r="D69" s="10">
+        <v>13620</v>
+      </c>
+      <c r="E69" s="11">
         <v>100.00</v>
       </c>
     </row>
-    <row r="69" ht="12" customHeight="1"/>
-    <row r="70" ht="14" customHeight="1">
-      <c r="A70" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-    </row>
-    <row r="71" ht="29" customHeight="1">
-      <c r="A71" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D71" s="9" t="s">
+    <row r="70" ht="12" customHeight="1"/>
+    <row r="71" ht="14" customHeight="1">
+      <c r="A71" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+    </row>
+    <row r="72" ht="29" customHeight="1">
+      <c r="A72" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B72" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E71" s="9" t="s">
+      <c r="C72" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="72" ht="14" customHeight="1">
-      <c r="A72" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B72" s="10">
-        <v>12554</v>
-      </c>
-      <c r="C72" s="11">
-        <v>92.17</v>
-      </c>
-      <c r="D72" s="10">
-        <v>12554</v>
-      </c>
-      <c r="E72" s="11">
-        <v>92.17</v>
+      <c r="D72" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="73" ht="14" customHeight="1">
       <c r="A73" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B73" s="10">
+        <v>12554</v>
+      </c>
+      <c r="C73" s="11">
+        <v>92.17</v>
+      </c>
+      <c r="D73" s="10">
+        <v>12554</v>
+      </c>
+      <c r="E73" s="11">
+        <v>92.17</v>
+      </c>
+    </row>
+    <row r="74" ht="14" customHeight="1">
+      <c r="A74" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B74" s="10">
         <v>1066</v>
       </c>
-      <c r="C73" s="11">
+      <c r="C74" s="11">
         <v>7.83</v>
       </c>
-      <c r="D73" s="10">
-        <v>13620</v>
-      </c>
-      <c r="E73" s="11">
+      <c r="D74" s="10">
+        <v>13620</v>
+      </c>
+      <c r="E74" s="11">
         <v>100.00</v>
       </c>
     </row>
-    <row r="74" ht="12" customHeight="1"/>
-    <row r="75" ht="14" customHeight="1">
-      <c r="A75" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-    </row>
-    <row r="76" ht="29" customHeight="1">
-      <c r="A76" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D76" s="9" t="s">
+    <row r="75" ht="12" customHeight="1"/>
+    <row r="76" ht="14" customHeight="1">
+      <c r="A76" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+    </row>
+    <row r="77" ht="29" customHeight="1">
+      <c r="A77" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B77" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E76" s="9" t="s">
+      <c r="C77" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="77" ht="14" customHeight="1">
-      <c r="A77" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B77" s="10">
-        <v>553</v>
-      </c>
-      <c r="C77" s="11">
-        <v>4.06</v>
-      </c>
-      <c r="D77" s="10">
-        <v>553</v>
-      </c>
-      <c r="E77" s="11">
-        <v>4.06</v>
+      <c r="D77" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="78" ht="14" customHeight="1">
       <c r="A78" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B78" s="10">
-        <v>5345</v>
+        <v>553</v>
       </c>
       <c r="C78" s="11">
-        <v>39.24</v>
+        <v>4.06</v>
       </c>
       <c r="D78" s="10">
-        <v>5898</v>
+        <v>553</v>
       </c>
       <c r="E78" s="11">
-        <v>43.30</v>
+        <v>4.06</v>
       </c>
     </row>
     <row r="79" ht="14" customHeight="1">
       <c r="A79" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B79" s="10">
-        <v>3266</v>
+        <v>5345</v>
       </c>
       <c r="C79" s="11">
-        <v>23.98</v>
+        <v>39.24</v>
       </c>
       <c r="D79" s="10">
-        <v>9164</v>
+        <v>5898</v>
       </c>
       <c r="E79" s="11">
-        <v>67.28</v>
+        <v>43.30</v>
       </c>
     </row>
     <row r="80" ht="14" customHeight="1">
       <c r="A80" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B80" s="10">
+        <v>3266</v>
+      </c>
+      <c r="C80" s="11">
+        <v>23.98</v>
+      </c>
+      <c r="D80" s="10">
+        <v>9164</v>
+      </c>
+      <c r="E80" s="11">
+        <v>67.28</v>
+      </c>
+    </row>
+    <row r="81" ht="14" customHeight="1">
+      <c r="A81" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B81" s="10">
         <v>4456</v>
       </c>
-      <c r="C80" s="11">
+      <c r="C81" s="11">
         <v>32.72</v>
       </c>
-      <c r="D80" s="10">
-        <v>13620</v>
-      </c>
-      <c r="E80" s="11">
+      <c r="D81" s="10">
+        <v>13620</v>
+      </c>
+      <c r="E81" s="11">
         <v>100.00</v>
       </c>
     </row>
-    <row r="81" ht="12" customHeight="1"/>
+    <row r="82" ht="12" customHeight="1"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A53:E53"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A63:E63"/>
-    <mergeCell ref="A70:E70"/>
-    <mergeCell ref="A75:E75"/>
-    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A64:E64"/>
+    <mergeCell ref="A71:E71"/>
+    <mergeCell ref="A76:E76"/>
+    <mergeCell ref="A27:I27"/>
   </mergeCells>
   <printOptions headings="0" horizontalCentered="0" verticalCentered="0" gridLines="0"/>
   <pageMargins left="0.05" right="0.05" top="0.5" bottom="0.5" header="0" footer="0"/>

</xml_diff>